<commit_message>
added chrome-remote and firefox-remote to the spreadsheet to allow it work with selenium grid/ hub docker
</commit_message>
<xml_diff>
--- a/Excel_Templates/Test_Suite_Template.xlsx
+++ b/Excel_Templates/Test_Suite_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19200"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19200" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Project_Name</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Headless</t>
+  </si>
+  <si>
+    <t>Chrome-Remote</t>
+  </si>
+  <si>
+    <t>Firefox-Remote</t>
   </si>
 </sst>
 </file>
@@ -625,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -702,7 +708,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$A$2:$A$14</xm:f>
+            <xm:f>Lists!$A$2:$A$16</xm:f>
           </x14:formula1>
           <xm:sqref>C8:C9</xm:sqref>
         </x14:dataValidation>
@@ -714,15 +720,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A6"/>
+  <dimension ref="A2:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -732,21 +738,31 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated test suite to include Chrome-Headless and Firefox-headless
</commit_message>
<xml_diff>
--- a/Excel_Templates/Test_Suite_Template.xlsx
+++ b/Excel_Templates/Test_Suite_Template.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Project_Name</t>
   </si>
@@ -72,13 +72,16 @@
     <t>Safari</t>
   </si>
   <si>
-    <t>Headless</t>
-  </si>
-  <si>
     <t>Chrome-Remote</t>
   </si>
   <si>
     <t>Firefox-Remote</t>
+  </si>
+  <si>
+    <t>Chrome-Headless</t>
+  </si>
+  <si>
+    <t>FireFox-Headless</t>
   </si>
 </sst>
 </file>
@@ -720,10 +723,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A8"/>
+  <dimension ref="A2:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -738,7 +741,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
@@ -748,7 +751,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
@@ -763,7 +766,12 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -772,12 +780,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008EB026D4FC24C9499CD13E6F13776440" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bde19c557e1184fdfae2ef1e0c5f05ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -891,16 +908,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9AA4BDC-0A1E-477B-A688-3C63CC63036F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78225F9A-721A-4D59-A0A0-AA4F79F57621}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -915,7 +931,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC8903CE-274A-40A9-9572-7A8439889D59}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -929,12 +945,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9AA4BDC-0A1E-477B-A688-3C63CC63036F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>